<commit_message>
oppdatert kursinfo for V26
</commit_message>
<xml_diff>
--- a/assets/orakeltjeneste.xlsx
+++ b/assets/orakeltjeneste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s12600\Documents\Work\projects\BED3\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\BED3\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D314DEDC-3DA5-48B2-B416-7AC10B5C3F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811BE5E6-423B-46A9-9F92-64ADF9B4B76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{C0B44EF9-4913-4C7F-926D-24A51F9A4763}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{C0B44EF9-4913-4C7F-926D-24A51F9A4763}"/>
   </bookViews>
   <sheets>
     <sheet name="Orakeltjeneste" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>Merknad</t>
   </si>
   <si>
-    <t>Innleveringssett har frist 25.04</t>
-  </si>
-  <si>
     <t>Andre påskedag</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>Himmelfartsdag</t>
+  </si>
+  <si>
+    <t>Innleveringssett har frist 17.04</t>
   </si>
 </sst>
 </file>
@@ -484,17 +484,17 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -520,7 +520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>17</v>
       </c>
@@ -528,16 +528,16 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>18</v>
       </c>
@@ -545,13 +545,13 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>19</v>
       </c>
@@ -559,10 +559,10 @@
         <v>9</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>20</v>
       </c>
@@ -570,19 +570,19 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>21</v>
       </c>
@@ -590,7 +590,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>22</v>
       </c>
@@ -598,10 +598,10 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
         <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>